<commit_message>
implementazione late e early fusion
</commit_message>
<xml_diff>
--- a/benchmark_results.xlsx
+++ b/benchmark_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1766,6 +1766,55 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Wav2Vec2 Phoneme</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Wav2Vec2</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Aug_Comb</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>34.6</v>
+      </c>
+      <c r="E28" t="n">
+        <v>65.40000000000001</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.5766</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.6059</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.8464</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.4904</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0.8512999999999999</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0.3444</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>